<commit_message>
add titles,description and source links
</commit_message>
<xml_diff>
--- a/etsy.xlsx
+++ b/etsy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yokai47\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yokai47\Documents\vscode\etsy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D5DA65-460E-4038-A914-80A1344070AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F730E94C-D48E-4312-9AA7-5E4944A6089A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{782A3891-46AD-4778-B162-B1E39679A610}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Category</t>
   </si>
@@ -59,33 +59,9 @@
     <t>Tags</t>
   </si>
   <si>
-    <t>assets</t>
-  </si>
-  <si>
-    <t>Jungle Animals Pack</t>
-  </si>
-  <si>
-    <t>Sea Animals Pack</t>
-  </si>
-  <si>
     <t>Dinosaurs Pack</t>
   </si>
   <si>
-    <t>Farm  Animals Pack</t>
-  </si>
-  <si>
-    <t>Forest  Animals Pack</t>
-  </si>
-  <si>
-    <t>Savana  Animals Pack</t>
-  </si>
-  <si>
-    <t>Desert  Animals Pack</t>
-  </si>
-  <si>
-    <t>Arctic  Animals Pack</t>
-  </si>
-  <si>
     <t>Birds Pack</t>
   </si>
   <si>
@@ -93,6 +69,52 @@
   </si>
   <si>
     <t>animal flashcards</t>
+  </si>
+  <si>
+    <t>Jungle Pack</t>
+  </si>
+  <si>
+    <t>Sea Pack</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Farm Pack</t>
+  </si>
+  <si>
+    <t>Forest Pack</t>
+  </si>
+  <si>
+    <t>Savana Pack</t>
+  </si>
+  <si>
+    <t>Arctic Pack</t>
+  </si>
+  <si>
+    <t>Desert Pack</t>
+  </si>
+  <si>
+    <t># Jungle Pack Flashcards 🐅🦧🦜
+Bring the jungle to life with this **digital printable flashcards pack**! The **Jungle Pack** includes **20 beautifully illustrated flashcards** featuring popular jungle animals like tigers, monkeys, elephants, parrots, and more. Each card comes with a **fun fact** to make learning **engaging, interactive, and educational** for kids ages 3+.
+## Perfect for:
+- Montessori activities  
+- Safari-themed classrooms  
+- Homeschool lessons  
+- Early childhood learning at home  
+## Features:
+- 20 high-quality **Jungle Animal Flashcards**  
+- **Instant digital download** (PDF format)  
+- Fun facts on each card to boost curiosity  
+- Printable at home, ready to cut and use  
+## Part of the Animal Flashcards Collection
+This pack is one of **10 themed packs** in our **Animal Flashcards Collection**, which also includes:  
+**Sea Pack, Dinosaurs Pack, Farm Pack, Forest Pack, Savana Pack, Desert Pack, Arctic Pack, Birds Pack, and Bugs Pack.** Collect them all to create a **full educational library** of animals from every environment!
+## How it Works:
+1. Purchase the listing  
+2. Download the PDF  
+3. Print at home and enjoy  
+Give your child a **fun and interactive way to learn about animals**, improve vocabulary, memory, and curiosity—all while having fun exploring the jungle!</t>
   </si>
 </sst>
 </file>
@@ -102,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +141,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC0CAF5"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,10 +241,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -225,10 +256,10 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -237,8 +268,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -585,21 +623,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8812C2E3-0A4A-4A05-AA82-3BA4786E7C67}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="94" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
@@ -624,7 +662,7 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -632,159 +670,230 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
-        <v>46034</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="b">
-        <v>0</v>
+        <v>46035</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>LEFT(C2, FIND(" ", C2 &amp; " ") - 1) &amp; " Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download"</f>
+        <v>Jungle Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="8" t="str">
+        <f>HYPERLINK("https://younes-alhyan.github.io/etsy/" &amp; SUBSTITUTE(LOWER(B2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(C2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(C2)," ","-") &amp; ".zip")</f>
+        <v>https://younes-alhyan.github.io/etsy/animal-flashcards/jungle-pack/jungle-pack.zip</v>
+      </c>
+      <c r="H2" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>46035</v>
+        <v>46036</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5" t="b">
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="str">
+        <f t="shared" ref="D3:D11" si="0">LEFT(C3, FIND(" ", C3 &amp; " ") - 1) &amp; " Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download"</f>
+        <v>Sea Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="8" t="str">
+        <f t="shared" ref="G3:G11" si="1">HYPERLINK("https://younes-alhyan.github.io/etsy/" &amp; SUBSTITUTE(LOWER(B3)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(C3)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(C3)," ","-") &amp; ".zip")</f>
+        <v>https://younes-alhyan.github.io/etsy//sea-pack/sea-pack.zip</v>
+      </c>
+      <c r="H3" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>46036</v>
+        <v>46037</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5" t="b">
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Dinosaurs Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//dinosaurs-pack/dinosaurs-pack.zip</v>
+      </c>
+      <c r="H4" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>46037</v>
+        <v>46038</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="b">
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Farm Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//farm-pack/farm-pack.zip</v>
+      </c>
+      <c r="H5" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>46038</v>
+        <v>46039</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="b">
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Forest Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//forest-pack/forest-pack.zip</v>
+      </c>
+      <c r="H6" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>46039</v>
+        <v>46040</v>
       </c>
       <c r="B7" s="6"/>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="b">
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Savana Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//savana-pack/savana-pack.zip</v>
+      </c>
+      <c r="H7" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>46040</v>
+        <v>46041</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="b">
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Desert Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//desert-pack/desert-pack.zip</v>
+      </c>
+      <c r="H8" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="3">
+        <v>46042</v>
+      </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5" t="b">
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Arctic Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//arctic-pack/arctic-pack.zip</v>
+      </c>
+      <c r="H9" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="3">
+        <v>46043</v>
+      </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5" t="b">
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Birds Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//birds-pack/birds-pack.zip</v>
+      </c>
+      <c r="H10" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="3">
+        <v>46044</v>
+      </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5" t="b">
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Bugs Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>https://younes-alhyan.github.io/etsy//bugs-pack/bugs-pack.zip</v>
+      </c>
+      <c r="H11" s="4" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
adjust text alignment and cell formatting
</commit_message>
<xml_diff>
--- a/etsy.xlsx
+++ b/etsy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yokai47\Documents\vscode\etsy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FE3096-3B76-4273-AFDA-B05F0392B2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F8EF0C-182A-48FE-BD26-91B0B6DE8710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{782A3891-46AD-4778-B162-B1E39679A610}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Category</t>
   </si>
@@ -343,9 +343,6 @@
   </si>
   <si>
     <t>animal flashcards, kids flashcards, printable learning, Montessori cards, educational cards, digital download, PDF flashcards, homeschool activities, preschool learning, birds flashcards, flying animals, avian creatures, early learning</t>
-  </si>
-  <si>
-    <t>animal flashcards, kids flashcards, printable learning, Montessori cards, educational cards, digital download, PDF flashcards, homeschool activities, preschool learning, bugs flashcards, insects learning, creepy crawlies, early learning</t>
   </si>
 </sst>
 </file>
@@ -857,7 +854,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="B2:F11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,8 +1084,8 @@
       <c r="D11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>36</v>
+      <c r="E11" s="9">
+        <v>0</v>
       </c>
       <c r="F11" s="10" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
fix typo in savanna pack name
</commit_message>
<xml_diff>
--- a/etsy.xlsx
+++ b/etsy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yokai47\Documents\vscode\etsy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F8EF0C-182A-48FE-BD26-91B0B6DE8710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7644B09-F844-4771-80F4-950485E02312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{782A3891-46AD-4778-B162-B1E39679A610}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{782A3891-46AD-4778-B162-B1E39679A610}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Category</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Forest Pack</t>
-  </si>
-  <si>
-    <t>Savana Pack</t>
   </si>
   <si>
     <t>Arctic Pack</t>
@@ -343,6 +340,12 @@
   </si>
   <si>
     <t>animal flashcards, kids flashcards, printable learning, Montessori cards, educational cards, digital download, PDF flashcards, homeschool activities, preschool learning, birds flashcards, flying animals, avian creatures, early learning</t>
+  </si>
+  <si>
+    <t>Savanna Pack</t>
+  </si>
+  <si>
+    <t>animal flashcards, kids flashcards, printable learning, Montessori cards, educational cards, digital download, PDF flashcards, homeschool activities, preschool learning, bugs flashcards, insects learning, creepy crawlies, early learning</t>
   </si>
 </sst>
 </file>
@@ -484,6 +487,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,15 +504,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -854,17 +857,17 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="102.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="210.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="82.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="191.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="2"/>
@@ -891,203 +894,203 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="str">
+      <c r="C2" s="5" t="str">
         <f>LEFT(B2, FIND(" ", B2 &amp; " ") - 1) &amp; " Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download"</f>
         <v>Jungle Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="10" t="str">
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="7" t="str">
         <f>HYPERLINK("https://younes-alhyan.github.io/etsy/" &amp; SUBSTITUTE(LOWER(A$2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B2)," ","-") &amp; ".zip")</f>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/jungle-pack/jungle-pack.zip</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="str">
+      <c r="C3" s="5" t="str">
         <f t="shared" ref="C3:C11" si="0">LEFT(B3, FIND(" ", B3 &amp; " ") - 1) &amp; " Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download"</f>
         <v>Sea Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="10" t="str">
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="7" t="str">
         <f t="shared" ref="F3:F11" si="1">HYPERLINK("https://younes-alhyan.github.io/etsy/" &amp; SUBSTITUTE(LOWER(A$2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B3)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B3)," ","-") &amp; ".zip")</f>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/sea-pack/sea-pack.zip</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="str">
+      <c r="C4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Dinosaurs Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="10" t="str">
-        <f t="shared" si="1"/>
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7" t="str">
+        <f>HYPERLINK("https://younes-alhyan.github.io/etsy/" &amp; SUBSTITUTE(LOWER(A$2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B4)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B4)," ","-") &amp; ".zip")</f>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/dinosaurs-pack/dinosaurs-pack.zip</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="str">
+      <c r="C5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Farm Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="10" t="str">
-        <f t="shared" si="1"/>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f>HYPERLINK("https://younes-alhyan.github.io/etsy/" &amp; SUBSTITUTE(LOWER(A$2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B5)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B5)," ","-") &amp; ".zip")</f>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/farm-pack/farm-pack.zip</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="str">
+      <c r="C6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Forest Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="10" t="str">
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/forest-pack/forest-pack.zip</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8" t="str">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>Savana Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="10" t="str">
+        <v>Savanna Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>https://younes-alhyan.github.io/etsy/animal-flashcards/savana-pack/savana-pack.zip</v>
+        <v>https://younes-alhyan.github.io/etsy/animal-flashcards/savanna-pack/savanna-pack.zip</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="str">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Desert Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="10" t="str">
-        <f t="shared" si="1"/>
+      <c r="D8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="7" t="str">
+        <f>HYPERLINK("https://younes-alhyan.github.io/etsy/" &amp; SUBSTITUTE(LOWER(A$2)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B8)," ","-") &amp; "/" &amp; SUBSTITUTE(LOWER(B8)," ","-") &amp; ".zip")</f>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/desert-pack/desert-pack.zip</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="str">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Arctic Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="10" t="str">
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/arctic-pack/arctic-pack.zip</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="8" t="str">
+      <c r="C10" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Birds Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="10" t="str">
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/birds-pack/birds-pack.zip</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="8" t="str">
+      <c r="C11" s="5" t="str">
         <f t="shared" si="0"/>
         <v>Bugs Animal Flashcards | Printable Kids Learning Cards | Montessori, Safari, Education, PDF Digital Download</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10" t="str">
+      <c r="D11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>https://younes-alhyan.github.io/etsy/animal-flashcards/bugs-pack/bugs-pack.zip</v>
       </c>

</xml_diff>